<commit_message>
Addeda Table updater form
</commit_message>
<xml_diff>
--- a/docs/Tissue to Block database.xlsx
+++ b/docs/Tissue to Block database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kristyp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Useful Documents-KP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="168">
   <si>
     <t>Specimen preparation</t>
   </si>
@@ -411,6 +411,132 @@
   </si>
   <si>
     <t>None- live tissue</t>
+  </si>
+  <si>
+    <t>p99</t>
+  </si>
+  <si>
+    <t>p96</t>
+  </si>
+  <si>
+    <t>H16.03.005</t>
+  </si>
+  <si>
+    <t>HSV_hEF1αG6s_P2A nls-dTom 6/28</t>
+  </si>
+  <si>
+    <t>HSV_hSyn1_EYFP 6/29</t>
+  </si>
+  <si>
+    <t>H16.06.008</t>
+  </si>
+  <si>
+    <t>H16.06.009</t>
+  </si>
+  <si>
+    <t>H16.06.010</t>
+  </si>
+  <si>
+    <t>HSV_hEF1α_EGFP</t>
+  </si>
+  <si>
+    <t>Acute slices</t>
+  </si>
+  <si>
+    <t>Day 0 cultured slice</t>
+  </si>
+  <si>
+    <t>cultured slice day 0</t>
+  </si>
+  <si>
+    <t>cultured slice day 1</t>
+  </si>
+  <si>
+    <t>cultured slice day 2</t>
+  </si>
+  <si>
+    <t>cultured slice day 3</t>
+  </si>
+  <si>
+    <t>cultured slice day 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acute slice </t>
+  </si>
+  <si>
+    <t>H16.06.011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSV_HEF1α EYFP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSV_DLX_GFP </t>
+  </si>
+  <si>
+    <t>Notched</t>
+  </si>
+  <si>
+    <t>p38</t>
+  </si>
+  <si>
+    <t>p62</t>
+  </si>
+  <si>
+    <t>p78</t>
+  </si>
+  <si>
+    <t>Chat tdT</t>
+  </si>
+  <si>
+    <t>NdnF tdT</t>
+  </si>
+  <si>
+    <t>Scnn1a_Tg2 tdT</t>
+  </si>
+  <si>
+    <t>Chrna2-Cre_OE25;Pvalb_2A_DreO;Ai66D</t>
+  </si>
+  <si>
+    <t>Nos1/sst/FlptdT</t>
+  </si>
+  <si>
+    <t>p55</t>
+  </si>
+  <si>
+    <t>Scnn1a Tg3 tdT</t>
+  </si>
+  <si>
+    <t>p56</t>
+  </si>
+  <si>
+    <t>p45</t>
+  </si>
+  <si>
+    <t>Htr3a tdT</t>
+  </si>
+  <si>
+    <t>Pvalb tdT</t>
+  </si>
+  <si>
+    <t>mouse acute slice</t>
+  </si>
+  <si>
+    <t>mouse decap scoop</t>
+  </si>
+  <si>
+    <t>none - not fixed</t>
+  </si>
+  <si>
+    <t>H16.03.007</t>
+  </si>
+  <si>
+    <t>full titer</t>
+  </si>
+  <si>
+    <t>1:10 dilution</t>
+  </si>
+  <si>
+    <t>Brainphys media - looks bad</t>
   </si>
 </sst>
 </file>
@@ -761,17 +887,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" customWidth="1"/>
     <col min="10" max="10" width="8.140625" customWidth="1"/>
@@ -2469,6 +2595,1277 @@
       </c>
       <c r="S35">
         <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>246934</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36">
+        <v>246934</v>
+      </c>
+      <c r="F36" s="5">
+        <v>42557</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36" s="5">
+        <v>42557</v>
+      </c>
+      <c r="M36" s="5">
+        <v>42563</v>
+      </c>
+      <c r="N36">
+        <v>3</v>
+      </c>
+      <c r="O36">
+        <v>4</v>
+      </c>
+      <c r="P36">
+        <v>3</v>
+      </c>
+      <c r="Q36">
+        <v>2</v>
+      </c>
+      <c r="R36">
+        <v>4</v>
+      </c>
+      <c r="S36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>246935</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37">
+        <v>246935</v>
+      </c>
+      <c r="F37" s="5">
+        <v>42557</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37" s="5">
+        <v>42557</v>
+      </c>
+      <c r="M37" s="5">
+        <v>42563</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+      <c r="O37">
+        <v>4</v>
+      </c>
+      <c r="P37">
+        <v>3</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37">
+        <v>4</v>
+      </c>
+      <c r="S37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>247514</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38">
+        <v>247514</v>
+      </c>
+      <c r="F38" s="5">
+        <v>42557</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38" s="5">
+        <v>42557</v>
+      </c>
+      <c r="M38" s="5">
+        <v>42563</v>
+      </c>
+      <c r="N38">
+        <v>3</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38">
+        <v>3</v>
+      </c>
+      <c r="Q38">
+        <v>2</v>
+      </c>
+      <c r="R38">
+        <v>4</v>
+      </c>
+      <c r="S38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>247516</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39">
+        <v>247516</v>
+      </c>
+      <c r="F39" s="5">
+        <v>42557</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39" s="5">
+        <v>42557</v>
+      </c>
+      <c r="M39" s="5">
+        <v>42563</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>4</v>
+      </c>
+      <c r="P39">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39">
+        <v>4</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" t="s">
+        <v>129</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40" s="5">
+        <v>42562</v>
+      </c>
+      <c r="M40" s="5">
+        <v>42563</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+      <c r="O40">
+        <v>4</v>
+      </c>
+      <c r="P40">
+        <v>3</v>
+      </c>
+      <c r="Q40">
+        <v>2</v>
+      </c>
+      <c r="R40">
+        <v>4</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
+        <v>130</v>
+      </c>
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41" s="5">
+        <v>42562</v>
+      </c>
+      <c r="M41" s="5">
+        <v>42563</v>
+      </c>
+      <c r="N41">
+        <v>3</v>
+      </c>
+      <c r="O41">
+        <v>4</v>
+      </c>
+      <c r="P41">
+        <v>3</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41">
+        <v>4</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42" s="5">
+        <v>42563</v>
+      </c>
+      <c r="M42" s="5">
+        <v>42584</v>
+      </c>
+      <c r="N42">
+        <v>3</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="P42">
+        <v>3</v>
+      </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="R42">
+        <v>4</v>
+      </c>
+      <c r="S42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+      <c r="L43" s="5">
+        <v>42564</v>
+      </c>
+      <c r="M43" s="5">
+        <v>42584</v>
+      </c>
+      <c r="N43">
+        <v>3</v>
+      </c>
+      <c r="O43">
+        <v>4</v>
+      </c>
+      <c r="P43">
+        <v>3</v>
+      </c>
+      <c r="Q43">
+        <v>2</v>
+      </c>
+      <c r="R43">
+        <v>4</v>
+      </c>
+      <c r="S43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+      <c r="M44" s="5">
+        <v>42584</v>
+      </c>
+      <c r="N44">
+        <v>3</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>3</v>
+      </c>
+      <c r="Q44">
+        <v>2</v>
+      </c>
+      <c r="R44">
+        <v>4</v>
+      </c>
+      <c r="S44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>134</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="M45" s="5">
+        <v>42584</v>
+      </c>
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>3</v>
+      </c>
+      <c r="Q45">
+        <v>2</v>
+      </c>
+      <c r="R45">
+        <v>4</v>
+      </c>
+      <c r="S45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46">
+        <v>14</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>4</v>
+      </c>
+      <c r="M46" s="5">
+        <v>42584</v>
+      </c>
+      <c r="N46">
+        <v>3</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>3</v>
+      </c>
+      <c r="Q46">
+        <v>2</v>
+      </c>
+      <c r="R46">
+        <v>4</v>
+      </c>
+      <c r="S46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47">
+        <v>9</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="M47" s="5">
+        <v>42584</v>
+      </c>
+      <c r="N47">
+        <v>3</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>3</v>
+      </c>
+      <c r="Q47">
+        <v>2</v>
+      </c>
+      <c r="R47">
+        <v>4</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48">
+        <v>15</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="M48" s="5">
+        <v>42612</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>3</v>
+      </c>
+      <c r="Q48">
+        <v>2</v>
+      </c>
+      <c r="R48">
+        <v>4</v>
+      </c>
+      <c r="S48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>146</v>
+      </c>
+      <c r="G49">
+        <v>16</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>4</v>
+      </c>
+      <c r="M49" s="5">
+        <v>42612</v>
+      </c>
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>3</v>
+      </c>
+      <c r="Q49">
+        <v>2</v>
+      </c>
+      <c r="R49">
+        <v>4</v>
+      </c>
+      <c r="S49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50">
+        <v>16</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>4</v>
+      </c>
+      <c r="M50" s="5">
+        <v>42612</v>
+      </c>
+      <c r="N50">
+        <v>3</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>3</v>
+      </c>
+      <c r="Q50">
+        <v>2</v>
+      </c>
+      <c r="R50">
+        <v>4</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>271152</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" t="s">
+        <v>147</v>
+      </c>
+      <c r="E51">
+        <v>271152</v>
+      </c>
+      <c r="F51" s="5">
+        <v>42599</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+      <c r="L51" s="5">
+        <v>42599</v>
+      </c>
+      <c r="M51" s="5">
+        <v>42606</v>
+      </c>
+      <c r="N51">
+        <v>3</v>
+      </c>
+      <c r="O51">
+        <v>4</v>
+      </c>
+      <c r="P51">
+        <v>3</v>
+      </c>
+      <c r="Q51">
+        <v>2</v>
+      </c>
+      <c r="R51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>263885</v>
+      </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52">
+        <v>263885</v>
+      </c>
+      <c r="F52" s="5">
+        <v>42599</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52" t="s">
+        <v>18</v>
+      </c>
+      <c r="K52">
+        <v>4</v>
+      </c>
+      <c r="L52" s="5">
+        <v>42599</v>
+      </c>
+      <c r="M52" s="5">
+        <v>42606</v>
+      </c>
+      <c r="N52">
+        <v>3</v>
+      </c>
+      <c r="O52">
+        <v>4</v>
+      </c>
+      <c r="P52">
+        <v>3</v>
+      </c>
+      <c r="Q52">
+        <v>2</v>
+      </c>
+      <c r="R52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>259292</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53">
+        <v>259292</v>
+      </c>
+      <c r="F53" s="5">
+        <v>42599</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53">
+        <v>4</v>
+      </c>
+      <c r="L53" s="5">
+        <v>42599</v>
+      </c>
+      <c r="M53" s="5">
+        <v>42606</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
+      </c>
+      <c r="O53">
+        <v>4</v>
+      </c>
+      <c r="P53">
+        <v>3</v>
+      </c>
+      <c r="Q53">
+        <v>2</v>
+      </c>
+      <c r="R53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>262849</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54">
+        <v>262849</v>
+      </c>
+      <c r="F54" s="5">
+        <v>42605</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54" t="s">
+        <v>18</v>
+      </c>
+      <c r="K54">
+        <v>4</v>
+      </c>
+      <c r="L54" s="5">
+        <v>42605</v>
+      </c>
+      <c r="M54" s="5">
+        <v>42612</v>
+      </c>
+      <c r="N54">
+        <v>3</v>
+      </c>
+      <c r="O54">
+        <v>4</v>
+      </c>
+      <c r="P54">
+        <v>3</v>
+      </c>
+      <c r="Q54">
+        <v>2</v>
+      </c>
+      <c r="R54">
+        <v>4</v>
+      </c>
+      <c r="S54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>270923</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" t="s">
+        <v>155</v>
+      </c>
+      <c r="E55">
+        <v>270923</v>
+      </c>
+      <c r="F55" s="5">
+        <v>42605</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55">
+        <v>4</v>
+      </c>
+      <c r="L55" s="5">
+        <v>42605</v>
+      </c>
+      <c r="M55" s="5">
+        <v>42612</v>
+      </c>
+      <c r="N55">
+        <v>3</v>
+      </c>
+      <c r="O55">
+        <v>4</v>
+      </c>
+      <c r="P55">
+        <v>3</v>
+      </c>
+      <c r="Q55">
+        <v>2</v>
+      </c>
+      <c r="R55">
+        <v>4</v>
+      </c>
+      <c r="S55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>268034</v>
+      </c>
+      <c r="B56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56">
+        <v>268034</v>
+      </c>
+      <c r="F56" s="5">
+        <v>42620</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56" s="5">
+        <v>42620</v>
+      </c>
+      <c r="M56" s="5">
+        <v>42622</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>4</v>
+      </c>
+      <c r="P56">
+        <v>3</v>
+      </c>
+      <c r="Q56">
+        <v>2</v>
+      </c>
+      <c r="R56">
+        <v>4</v>
+      </c>
+      <c r="S56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>267682</v>
+      </c>
+      <c r="B57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57">
+        <v>267682</v>
+      </c>
+      <c r="F57" s="5">
+        <v>42620</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>3</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57" s="5">
+        <v>42620</v>
+      </c>
+      <c r="M57" s="5">
+        <v>42622</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>4</v>
+      </c>
+      <c r="P57">
+        <v>3</v>
+      </c>
+      <c r="Q57">
+        <v>2</v>
+      </c>
+      <c r="R57">
+        <v>4</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>270009</v>
+      </c>
+      <c r="B58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" t="s">
+        <v>160</v>
+      </c>
+      <c r="D58" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58">
+        <v>270009</v>
+      </c>
+      <c r="F58" s="5">
+        <v>42620</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58" s="5">
+        <v>42620</v>
+      </c>
+      <c r="M58" s="5">
+        <v>42622</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>4</v>
+      </c>
+      <c r="P58">
+        <v>3</v>
+      </c>
+      <c r="Q58">
+        <v>2</v>
+      </c>
+      <c r="R58">
+        <v>4</v>
+      </c>
+      <c r="S58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
+      <c r="M59" s="5">
+        <v>42626</v>
+      </c>
+      <c r="N59">
+        <v>3</v>
+      </c>
+      <c r="O59">
+        <v>4</v>
+      </c>
+      <c r="P59">
+        <v>3</v>
+      </c>
+      <c r="Q59">
+        <v>2</v>
+      </c>
+      <c r="R59">
+        <v>4</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>164</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" t="s">
+        <v>166</v>
+      </c>
+      <c r="G60">
+        <v>6</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>4</v>
+      </c>
+      <c r="M60" s="5">
+        <v>42626</v>
+      </c>
+      <c r="N60">
+        <v>3</v>
+      </c>
+      <c r="O60">
+        <v>4</v>
+      </c>
+      <c r="P60">
+        <v>3</v>
+      </c>
+      <c r="Q60">
+        <v>2</v>
+      </c>
+      <c r="R60">
+        <v>4</v>
+      </c>
+      <c r="S60">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2562,10 +3959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2652,6 +4049,70 @@
       </c>
       <c r="B10" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2727,7 +4188,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2774,6 +4235,14 @@
       </c>
       <c r="B5" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Got excel data imported into database
</commit_message>
<xml_diff>
--- a/docs/Tissue to Block database.xlsx
+++ b/docs/Tissue to Block database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Useful Documents-KP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\atDB\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15420" windowHeight="10935" tabRatio="746"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15420" windowHeight="10935" tabRatio="920"/>
   </bookViews>
   <sheets>
     <sheet name="Specimen List" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="169">
   <si>
     <t>Specimen preparation</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>Brainphys media - looks bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -611,8 +614,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -889,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3874,7 +3905,7 @@
     <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3883,7 +3914,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3962,7 +3993,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4126,7 +4157,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4188,7 +4219,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4263,7 +4294,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -4485,7 +4516,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -4555,6 +4586,11 @@
       </c>
       <c r="B9" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>